<commit_message>
Changes in one cell
</commit_message>
<xml_diff>
--- a/Song_list.xlsx
+++ b/Song_list.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BA3BF8C7-336B-4AED-B8AA-1620FEAEDC4A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,15 +19,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Prueba</t>
   </si>
+  <si>
+    <t>Cambiamos</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -339,16 +341,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>